<commit_message>
Atualização na planilha de Backlog.
Correção de erros nos requisitos do backlog.
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bandtec\TI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>RA</t>
   </si>
@@ -108,73 +108,46 @@
     <t>Classificação</t>
   </si>
   <si>
-    <t>RF1</t>
-  </si>
-  <si>
-    <t>O software deve permitir que o administrador efetue a manutenção (consulta, inclusão, exclusão e alteração) do estacionamento.</t>
-  </si>
-  <si>
     <t>Essencial</t>
   </si>
   <si>
     <t>Funcional</t>
   </si>
   <si>
-    <t>RF2</t>
-  </si>
-  <si>
-    <t>O software deve permitir que o usuario solicite a consulta das vagas.</t>
-  </si>
-  <si>
-    <t>RF3</t>
-  </si>
-  <si>
-    <t>O software deve permitir que o usuario gere relatorios atraves dos dados obtidos.</t>
-  </si>
-  <si>
-    <t>RF4</t>
-  </si>
-  <si>
-    <t>O software deve permitir que o administrador gere relatorios atraves dos dados obtidos.</t>
-  </si>
-  <si>
     <t>Importante</t>
   </si>
   <si>
-    <t>RF5</t>
-  </si>
-  <si>
-    <t>O software deve gerar graficos atraves dos dados obtidos.</t>
-  </si>
-  <si>
-    <t>Não Funcional</t>
-  </si>
-  <si>
-    <t>RF6</t>
-  </si>
-  <si>
-    <t>O software deve receber dados pelo sensor do arduino.</t>
-  </si>
-  <si>
-    <t>RF7</t>
-  </si>
-  <si>
-    <t>O arduino deve ter sensor de obstaculo.</t>
-  </si>
-  <si>
     <t>Beatriz Barbosa</t>
   </si>
   <si>
     <t>01201137</t>
   </si>
   <si>
-    <t>RF8</t>
-  </si>
-  <si>
-    <t>O software deve permitir que o usuario comum solicite a consulta de vagas disponiveis no momento</t>
-  </si>
-  <si>
-    <t>Desejavel</t>
+    <t>Desejável</t>
+  </si>
+  <si>
+    <t>O software deve permitir que o administrador efetue a manutenção (consulta, inclusão, exclusão e alteração) dos dados.</t>
+  </si>
+  <si>
+    <t>O software deve permitir que o usuário solicite a consulta das vagas.</t>
+  </si>
+  <si>
+    <t>O software deve permitir que o usuário gere relatorios atraves dos dados obtidos.</t>
+  </si>
+  <si>
+    <t>O software deve permitir que o administrador gere relatórios através dos dados obtidos.</t>
+  </si>
+  <si>
+    <t>O software deve gerar gráficos através dos dados obtidos.</t>
+  </si>
+  <si>
+    <t>O software deve receber dados pelo sensor do arduíno.</t>
+  </si>
+  <si>
+    <t>O arduíno deve ter sensor de obstáculo.</t>
+  </si>
+  <si>
+    <t>O software deve permitir que o usuário comum solicite a consulta de vagas disponíveis no momento.</t>
   </si>
 </sst>
 </file>
@@ -278,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -295,6 +268,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1012,7 +994,7 @@
   <dimension ref="B2:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1031,10 +1013,10 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -1078,7 +1060,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1092,117 +1074,117 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="14">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>19</v>
+      <c r="B12" s="14">
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>21</v>
+      <c r="B13" s="14">
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>23</v>
+      <c r="B14" s="14">
+        <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="14">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="14">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="15">
+        <v>7</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="D17" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>35</v>
+      <c r="B18" s="14">
+        <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1262,21 +1244,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9BC80282CCA404AA1CD1CA861A2963D" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4d0a986244f0c450349ad09cdebecbb2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c4830a68-a8b0-4951-a620-6963d0f88529" xmlns:ns4="8883472b-a884-4206-9b1d-0a9e1a4d759c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd11ff14991a2a7c4b2bd50579d584c1" ns3:_="" ns4:_="">
     <xsd:import namespace="c4830a68-a8b0-4951-a620-6963d0f88529"/>
@@ -1485,24 +1452,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7A69715-2BF2-473E-A417-403290B48624}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6307CC5C-35AE-4BF6-AB1C-CA68C1295C47}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3905A48-2209-475D-B89F-4D2CCA4D7509}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1519,4 +1484,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6307CC5C-35AE-4BF6-AB1C-CA68C1295C47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7A69715-2BF2-473E-A417-403290B48624}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>